<commit_message>
Push initial changes for ShiftRow and corresponding changes to ProtectedArea.java and MoveController.java. This is first iteration and there will likely be some bugs that I will resolve in the next checkin.
</commit_message>
<xml_diff>
--- a/CyberPoetrySlam/Task3_Breakdown.xlsx
+++ b/CyberPoetrySlam/Task3_Breakdown.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="145" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Task3-Breakdown" sheetId="1" state="visible" r:id="rId2"/>
@@ -124,6 +124,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -145,6 +146,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -482,7 +484,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -781,7 +783,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>